<commit_message>
symbol table in Excel; other minor tweaks
</commit_message>
<xml_diff>
--- a/SymbolTable.xlsx
+++ b/SymbolTable.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="130">
   <si>
     <t>$y$</t>
   </si>
@@ -325,14 +325,147 @@
   </si>
   <si>
     <t>interannual variation in herring yield</t>
+  </si>
+  <si>
+    <t>$SSB_{MSY}^P$</t>
+  </si>
+  <si>
+    <t>predator spawning stock biomass at maximum sustainable yield</t>
+  </si>
+  <si>
+    <t>$GR$</t>
+  </si>
+  <si>
+    <t>gross revenue</t>
+  </si>
+  <si>
+    <t>$NR$</t>
+  </si>
+  <si>
+    <t>net operating revenues</t>
+  </si>
+  <si>
+    <t>$i$</t>
+  </si>
+  <si>
+    <t>$q$</t>
+  </si>
+  <si>
+    <t>quantity landed</t>
+  </si>
+  <si>
+    <t>$c$</t>
+  </si>
+  <si>
+    <t>cost function</t>
+  </si>
+  <si>
+    <t>$p$</t>
+  </si>
+  <si>
+    <t>function relating landings to prices</t>
+  </si>
+  <si>
+    <t>$t$</t>
+  </si>
+  <si>
+    <t>denotes trawl fishery in economic model</t>
+  </si>
+  <si>
+    <t>$s$</t>
+  </si>
+  <si>
+    <t>denotes purse seine fishery in economic model</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">fleet (trawl, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">t, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">or purse seine, </t>
+    </r>
+    <r>
+      <rPr>
+        <i/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>s</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>)</t>
+    </r>
+  </si>
+  <si>
+    <t>$a_i$</t>
+  </si>
+  <si>
+    <t>parameter of price and landing model</t>
+  </si>
+  <si>
+    <t>$b$</t>
+  </si>
+  <si>
+    <t>$\gamma$</t>
+  </si>
+  <si>
+    <t>$\alpha$</t>
+  </si>
+  <si>
+    <t>$\theta_i$</t>
+  </si>
+  <si>
+    <t>$\beta$</t>
+  </si>
+  <si>
+    <t>$\xi$</t>
+  </si>
+  <si>
+    <t>parameter of economic stationarity metric</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -663,10 +796,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B53"/>
+  <dimension ref="A2:B69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="A54" sqref="A54"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E43" sqref="E43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1088,6 +1221,134 @@
       </c>
       <c r="B53" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" t="s">
+        <v>103</v>
+      </c>
+      <c r="B54" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" t="s">
+        <v>105</v>
+      </c>
+      <c r="B55" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A56" t="s">
+        <v>107</v>
+      </c>
+      <c r="B56" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A57" t="s">
+        <v>109</v>
+      </c>
+      <c r="B57" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A58" t="s">
+        <v>110</v>
+      </c>
+      <c r="B58" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A59" t="s">
+        <v>112</v>
+      </c>
+      <c r="B59" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>114</v>
+      </c>
+      <c r="B60" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>116</v>
+      </c>
+      <c r="B61" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A62" t="s">
+        <v>118</v>
+      </c>
+      <c r="B62" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A63" t="s">
+        <v>121</v>
+      </c>
+      <c r="B63" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A64" t="s">
+        <v>123</v>
+      </c>
+      <c r="B64" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" t="s">
+        <v>124</v>
+      </c>
+      <c r="B65" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" t="s">
+        <v>125</v>
+      </c>
+      <c r="B66" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>126</v>
+      </c>
+      <c r="B67" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>127</v>
+      </c>
+      <c r="B68" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" t="s">
+        <v>128</v>
+      </c>
+      <c r="B69" t="s">
+        <v>129</v>
       </c>
     </row>
   </sheetData>

</xml_diff>